<commit_message>
Guid pattern corrected to hhhhhhhh-hhhh-hhhh-hhhh-hhhhhhhhhhhh to fit RVL requirements
</commit_message>
<xml_diff>
--- a/PatternMatching/Main.rvl.xlsx
+++ b/PatternMatching/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="50">
   <si>
     <t>Flow</t>
   </si>
@@ -894,7 +894,7 @@
         <v>11</v>
       </c>
       <c r="G19" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20">
@@ -973,7 +973,7 @@
         <v>11</v>
       </c>
       <c r="G24" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25">
@@ -1049,7 +1049,7 @@
         <v>11</v>
       </c>
       <c r="G29" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30">
@@ -1125,7 +1125,7 @@
         <v>11</v>
       </c>
       <c r="G34" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35">

</xml_diff>